<commit_message>
Finished on the web api side.
</commit_message>
<xml_diff>
--- a/Docs/Western Mutual Policy.xlsx
+++ b/Docs/Western Mutual Policy.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Jobs\Western Mutual\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88A00B12-D9DE-4BBA-8A53-868179FACA72}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6C87695-89E5-404C-909C-56763F728A82}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32811" yWindow="-3240" windowWidth="33120" windowHeight="18120" xr2:uid="{620781F5-94F4-49F3-B728-3238B86E78C0}"/>
+    <workbookView xWindow="40183" yWindow="-2434" windowWidth="22783" windowHeight="17280" xr2:uid="{620781F5-94F4-49F3-B728-3238B86E78C0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="76">
   <si>
     <t>Policy</t>
   </si>
@@ -156,9 +156,6 @@
     <t>Freddie Espiritu</t>
   </si>
   <si>
-    <t>Teresa Espiritu</t>
-  </si>
-  <si>
     <t>Coverages</t>
   </si>
   <si>
@@ -223,6 +220,39 @@
   </si>
   <si>
     <t>- POST  /save</t>
+  </si>
+  <si>
+    <t>UI</t>
+  </si>
+  <si>
+    <t>Landing page</t>
+  </si>
+  <si>
+    <t>- Display view table</t>
+  </si>
+  <si>
+    <t>- Create a view model</t>
+  </si>
+  <si>
+    <t>(Edit button)</t>
+  </si>
+  <si>
+    <t>(Add button)</t>
+  </si>
+  <si>
+    <t>Policy page</t>
+  </si>
+  <si>
+    <t>- GET Lookup</t>
+  </si>
+  <si>
+    <t>- Endpoints</t>
+  </si>
+  <si>
+    <t>Coverage1, Coverage2</t>
+  </si>
+  <si>
+    <t>Coverage4, Coverage5</t>
   </si>
 </sst>
 </file>
@@ -238,7 +268,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -263,6 +293,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -276,7 +312,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -284,6 +320,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -598,10 +635,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2D2A75A-3256-44E9-ADF1-81A46B6C7CEB}">
-  <dimension ref="A1:N54"/>
+  <dimension ref="A1:O90"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30:C30"/>
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -611,19 +648,23 @@
     <col min="10" max="10" width="15.08984375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="14" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="14" customWidth="1"/>
-    <col min="13" max="13" width="10.6328125" customWidth="1"/>
+    <col min="13" max="13" width="22" customWidth="1"/>
     <col min="14" max="14" width="9" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="H1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="I1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
@@ -649,13 +690,13 @@
         <v>35</v>
       </c>
       <c r="M2" t="s">
+        <v>43</v>
+      </c>
+      <c r="N2" t="s">
         <v>44</v>
       </c>
-      <c r="N2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>1</v>
       </c>
@@ -681,14 +722,17 @@
         <v>36</v>
       </c>
       <c r="M3" t="s">
-        <v>18</v>
+        <v>74</v>
       </c>
       <c r="N3">
         <f>(1066000*0.11)+30</f>
         <v>117290</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>2</v>
       </c>
@@ -699,82 +743,37 @@
         <v>37</v>
       </c>
       <c r="H4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J4" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="K4" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="L4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="M4" t="s">
-        <v>29</v>
+        <v>75</v>
       </c>
       <c r="N4">
-        <f>(1066000*0.11)+30</f>
-        <v>117290</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="H5">
-        <v>2</v>
-      </c>
-      <c r="I5">
-        <v>2</v>
-      </c>
-      <c r="J5" t="s">
-        <v>13</v>
-      </c>
-      <c r="K5" t="s">
-        <v>47</v>
-      </c>
-      <c r="L5" t="s">
-        <v>37</v>
-      </c>
-      <c r="M5" t="s">
-        <v>31</v>
-      </c>
-      <c r="N5">
         <f>(500000*0.1)+70</f>
         <v>50070</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="H6">
-        <v>2</v>
-      </c>
-      <c r="I6">
-        <v>2</v>
-      </c>
-      <c r="J6" t="s">
-        <v>13</v>
-      </c>
-      <c r="K6" t="s">
-        <v>47</v>
-      </c>
-      <c r="L6" t="s">
-        <v>37</v>
-      </c>
-      <c r="M6" t="s">
-        <v>32</v>
-      </c>
-      <c r="N6">
-        <f>(500000*0.1)+70</f>
-        <v>50070</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A8" s="6" t="s">
         <v>1</v>
       </c>
@@ -788,7 +787,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>1</v>
       </c>
@@ -802,7 +801,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>2</v>
       </c>
@@ -816,7 +815,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>3</v>
       </c>
@@ -830,17 +829,30 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="J12" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="J13" s="5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="J14" s="5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A15" s="6" t="s">
         <v>1</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C15" s="6" t="s">
         <v>10</v>
@@ -849,10 +861,13 @@
         <v>22</v>
       </c>
       <c r="F15" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
+        <v>47</v>
+      </c>
+      <c r="J15" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>1</v>
       </c>
@@ -866,10 +881,10 @@
         <v>23</v>
       </c>
       <c r="F16" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>2</v>
       </c>
@@ -883,15 +898,20 @@
         <v>21</v>
       </c>
       <c r="F17" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="J19" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A20" s="7" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A21" s="6" t="s">
         <v>1</v>
       </c>
@@ -902,7 +922,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>1</v>
       </c>
@@ -913,7 +933,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>2</v>
       </c>
@@ -923,11 +943,8 @@
       <c r="C23" s="1">
         <v>20</v>
       </c>
-      <c r="H23" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>3</v>
       </c>
@@ -938,7 +955,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>4</v>
       </c>
@@ -948,11 +965,8 @@
       <c r="C25" s="3">
         <v>40</v>
       </c>
-      <c r="H25" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>5</v>
       </c>
@@ -962,24 +976,13 @@
       <c r="C26" s="4">
         <v>50</v>
       </c>
-      <c r="H26" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="H28" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A29" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="H29" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A30" s="6" t="s">
         <v>1</v>
       </c>
@@ -990,7 +993,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>1</v>
       </c>
@@ -1001,7 +1004,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>2</v>
       </c>
@@ -1011,32 +1014,13 @@
       <c r="C32">
         <v>1</v>
       </c>
-      <c r="H32" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="H33" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="H34" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>38</v>
       </c>
-      <c r="H35" t="s">
-        <v>56</v>
-      </c>
-      <c r="I35" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" s="6" t="s">
         <v>1</v>
       </c>
@@ -1046,14 +1030,8 @@
       <c r="C36" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="H36" t="s">
-        <v>56</v>
-      </c>
-      <c r="I36" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>1</v>
       </c>
@@ -1063,14 +1041,8 @@
       <c r="C37">
         <v>1</v>
       </c>
-      <c r="H37" t="s">
-        <v>56</v>
-      </c>
-      <c r="I37" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>2</v>
       </c>
@@ -1080,14 +1052,8 @@
       <c r="C38">
         <v>2</v>
       </c>
-      <c r="H38" t="s">
-        <v>56</v>
-      </c>
-      <c r="I38" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>3</v>
       </c>
@@ -1098,7 +1064,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>4</v>
       </c>
@@ -1109,23 +1075,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="H41" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A42" t="s">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A42" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="H42" t="s">
-        <v>57</v>
-      </c>
-      <c r="J42" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" s="6" t="s">
         <v>1</v>
       </c>
@@ -1136,11 +1091,8 @@
         <v>17</v>
       </c>
       <c r="D43" s="6"/>
-      <c r="H43" s="5" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>1</v>
       </c>
@@ -1150,11 +1102,8 @@
       <c r="C44" t="s">
         <v>25</v>
       </c>
-      <c r="H44" s="5" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>2</v>
       </c>
@@ -1165,7 +1114,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>3</v>
       </c>
@@ -1176,34 +1125,139 @@
         <v>27</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="H47" t="s">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
+        <v>56</v>
+      </c>
+      <c r="C56" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A57" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A58" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A60" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A61" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A63" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A64" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A67" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A68" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A69" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A70" t="s">
+        <v>55</v>
+      </c>
+      <c r="B70" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A71" t="s">
+        <v>55</v>
+      </c>
+      <c r="B71" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A72" t="s">
+        <v>55</v>
+      </c>
+      <c r="B72" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A73" t="s">
+        <v>55</v>
+      </c>
+      <c r="B73" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A82" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A83" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="H48" t="s">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A84" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="49" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H49" t="s">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A87" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="52" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H52" t="s">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A88" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A89" s="5" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="53" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H53" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H54" s="5" t="s">
-        <v>65</v>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A90" s="5" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>